<commit_message>
Added CopyToExcel in TetUtil with Override
</commit_message>
<xml_diff>
--- a/src/main/java/com/elevate/qa/testData/ProgramList.xlsx
+++ b/src/main/java/com/elevate/qa/testData/ProgramList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\komal\eclipse-workspace\POMFunctional\src\main\java\com\elevate\qa\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{241FEC29-228B-4A0D-A031-54D2248B2E1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F19C569D-6319-40F3-BECA-0A06C305BE86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{92E6C001-1927-4CC3-83BD-C59D153128C4}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Program Name</t>
   </si>
@@ -200,24 +200,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
@@ -550,7 +534,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -558,10 +544,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="19">
+      <c r="A1" t="s" s="3">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="20">
+      <c r="B1" t="s" s="4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Completed all AddNewSchoolPage test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/elevate/qa/testData/ProgramList.xlsx
+++ b/src/main/java/com/elevate/qa/testData/ProgramList.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
   <si>
     <t>Program Name</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>Yeager Middle School - Georgia Science 7th - UAT</t>
+  </si>
+  <si>
+    <t>Artificial Intelligence</t>
+  </si>
+  <si>
+    <t>LProgram1</t>
   </si>
 </sst>
 </file>
@@ -200,8 +206,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
@@ -532,7 +542,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D43"/>
@@ -544,10 +554,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="3">
+      <c r="A1" t="s" s="7">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="4">
+      <c r="B1" t="s" s="8">
         <v>1</v>
       </c>
     </row>
@@ -608,87 +618,87 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
@@ -698,66 +708,71 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented retry logic for all failed test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/elevate/qa/testData/ProgramList.xlsx
+++ b/src/main/java/com/elevate/qa/testData/ProgramList.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="45">
   <si>
     <t>Program Name</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>LProgram1</t>
+  </si>
+  <si>
+    <t>Demo 1</t>
+  </si>
+  <si>
+    <t>Importabc</t>
   </si>
 </sst>
 </file>
@@ -206,8 +212,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="true"/>
@@ -542,7 +552,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D43"/>
@@ -554,10 +564,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="11">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="8">
+      <c r="B1" t="s" s="12">
         <v>1</v>
       </c>
     </row>
@@ -653,126 +663,136 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>